<commit_message>
household and census data combined
</commit_message>
<xml_diff>
--- a/workplan.xlsx
+++ b/workplan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bisma\project2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D1A1C006-3DC8-464A-B3C9-1CE7F87D5172}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70652C0B-A9FD-4398-BF6A-66C23B66FE20}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20640" yWindow="600" windowWidth="15864" windowHeight="15708" activeTab="1" xr2:uid="{E6A7FF9F-FB40-4F68-A184-29DD4D337BCD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="17496" activeTab="1" xr2:uid="{E6A7FF9F-FB40-4F68-A184-29DD4D337BCD}"/>
   </bookViews>
   <sheets>
     <sheet name="Structure" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="Page 3" sheetId="4" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet5!$A$1:$C$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet5!$A$1:$E$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="40">
   <si>
     <t>Client</t>
   </si>
@@ -119,9 +119,6 @@
     <t>app.py (flask) revision + update</t>
   </si>
   <si>
-    <t>transfar pandas sqlalchemy code to VS code</t>
-  </si>
-  <si>
     <t>Caitilin</t>
   </si>
   <si>
@@ -156,6 +153,27 @@
   </si>
   <si>
     <t>content for webpages</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>census, salaries, incomes done</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>combine census tracts + income notebooks</t>
+  </si>
+  <si>
+    <t>merge census table + income table =&gt; load to db</t>
+  </si>
+  <si>
+    <t>Everyone</t>
   </si>
 </sst>
 </file>
@@ -1252,20 +1270,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDB243B8-CB1F-42A2-8BA8-88782C607173}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:E15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="39.77734375" customWidth="1"/>
+    <col min="1" max="1" width="42.44140625" customWidth="1"/>
     <col min="2" max="2" width="37" customWidth="1"/>
-    <col min="3" max="3" width="22.5546875" customWidth="1"/>
+    <col min="3" max="4" width="16.77734375" customWidth="1"/>
+    <col min="5" max="5" width="54.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>14</v>
       </c>
@@ -1275,8 +1294,14 @@
       <c r="C1" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -1286,108 +1311,143 @@
       <c r="C2" s="4">
         <v>44314</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D2" s="4"/>
+      <c r="E2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" t="s">
         <v>21</v>
       </c>
-      <c r="B3" t="s">
+      <c r="D4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" t="s">
+        <v>23</v>
+      </c>
+      <c r="C6" s="4">
+        <v>44319</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>23</v>
-      </c>
       <c r="B7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+      <c r="C7" s="4">
+        <v>44319</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>26</v>
       </c>
       <c r="B8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>27</v>
       </c>
       <c r="B9" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C9" s="4">
+        <v>44314</v>
+      </c>
+      <c r="D9" s="4"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>28</v>
       </c>
       <c r="B10" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="4">
-        <v>44314</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>29</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>30</v>
       </c>
       <c r="B12" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="C12" s="4">
+        <v>44321</v>
+      </c>
+      <c r="D12" s="4"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" t="s">
         <v>31</v>
       </c>
-      <c r="B13" t="s">
-        <v>32</v>
-      </c>
-      <c r="C13" s="4">
-        <v>44321</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="B14" t="s">
-        <v>32</v>
+        <v>24</v>
+      </c>
+      <c r="C14" s="4">
+        <v>44314</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="4">
+        <v>44314</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C1" xr:uid="{8CF1B49C-8CD1-4BAC-89C6-E39A97F58E5F}"/>
+  <autoFilter ref="A1:E1" xr:uid="{8E1BA738-CAC9-4A01-BCDA-598CCB1E92A0}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>